<commit_message>
Ajout de nouveaux produits et mise à jour des données initiales dans le système de gestion de stock. Amélioration de la fonction de recherche pour gérer les références en tant que chaînes de caractères. Réorganisation de l'interface utilisateur pour faciliter l'ajout rapide de produits au panier, avec une section de recherche améliorée et un scanner externe. Suppression des fichiers d'historique et de demandes obsolètes.
</commit_message>
<xml_diff>
--- a/data/inventaire.xlsx
+++ b/data/inventaire.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,32 +451,32 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Stock_Min</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Stock_Max</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Emplacement</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Fournisseur</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Date_Entree</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Prix_Unitaire</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Stock_Min</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Stock_Max</t>
         </is>
       </c>
     </row>
@@ -486,37 +486,35 @@
           <t>Tournevis cruciforme</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>TS001</t>
-        </is>
+      <c r="B2" t="n">
+        <v>8473926150</v>
       </c>
       <c r="C2" t="n">
-        <v>30</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Atelier B</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+        <v>50</v>
+      </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Atelier A</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Fournisseur A</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>2024-03-15</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>15.99</v>
-      </c>
-      <c r="H2" t="n">
-        <v>10</v>
-      </c>
-      <c r="I2" t="n">
-        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -525,37 +523,35 @@
           <t>Marteau 500g</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MH001</t>
-        </is>
+      <c r="B3" t="n">
+        <v>2938475610</v>
       </c>
       <c r="C3" t="n">
-        <v>29</v>
-      </c>
-      <c r="D3" t="inlineStr">
+        <v>30</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>50</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Atelier B</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Fournisseur B</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>2024-03-14</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>25.5</v>
-      </c>
-      <c r="H3" t="n">
-        <v>10</v>
-      </c>
-      <c r="I3" t="n">
-        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -564,37 +560,35 @@
           <t>Perceuse sans fil</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>PS001</t>
-        </is>
+      <c r="B4" t="n">
+        <v>9182736450</v>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
-      </c>
-      <c r="D4" t="inlineStr">
+        <v>15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Atelier A</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Fournisseur C</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>2024-03-13</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>89.98999999999999</v>
-      </c>
-      <c r="H4" t="n">
-        <v>5</v>
-      </c>
-      <c r="I4" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -603,37 +597,35 @@
           <t>Vis 6x50mm</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>V001</t>
-        </is>
+      <c r="B5" t="n">
+        <v>5647382910</v>
       </c>
       <c r="C5" t="n">
-        <v>1226</v>
-      </c>
-      <c r="D5" t="inlineStr">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>Stockage</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Fournisseur A</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>2024-03-12</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>0.15</v>
-      </c>
-      <c r="H5" t="n">
-        <v>500</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1200</v>
       </c>
     </row>
     <row r="6">
@@ -642,76 +634,405 @@
           <t>Clé à molette</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>CM001</t>
-        </is>
+      <c r="B6" t="n">
+        <v>1928374650</v>
       </c>
       <c r="C6" t="n">
-        <v>42</v>
-      </c>
-      <c r="D6" t="inlineStr">
+        <v>25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Atelier B</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Fournisseur B</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>2024-03-11</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>12.75</v>
-      </c>
-      <c r="H6" t="n">
-        <v>10</v>
-      </c>
-      <c r="I6" t="n">
-        <v>45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Parclose</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>102938475738883</t>
-        </is>
+          <t>Scie circulaire</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6574839201</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
-      </c>
-      <c r="D7" t="inlineStr">
+        <v>20</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Atelier A</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Fournisseur C</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-03-10</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>129.99</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ponceuse</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3847562910</v>
+      </c>
+      <c r="C8" t="n">
+        <v>35</v>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="n">
+        <v>70</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Atelier B</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Fournisseur A</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-03-09</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>79.98999999999999</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Niveau à bulle</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4758392016</v>
+      </c>
+      <c r="C9" t="n">
+        <v>40</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>80</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Atelier A</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Fournisseur B</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-03-08</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mètre ruban</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>8392017465</v>
+      </c>
+      <c r="C10" t="n">
+        <v>60</v>
+      </c>
+      <c r="D10" t="n">
+        <v>15</v>
+      </c>
+      <c r="E10" t="n">
+        <v>120</v>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>Stockage</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Fournisseur C</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-03-07</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Pince coupante</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>7465839201</v>
+      </c>
+      <c r="C11" t="n">
+        <v>45</v>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>90</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Atelier B</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Fournisseur A</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-03-06</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tournevis plat</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2837465910</v>
+      </c>
+      <c r="C12" t="n">
+        <v>55</v>
+      </c>
+      <c r="D12" t="n">
+        <v>12</v>
+      </c>
+      <c r="E12" t="n">
+        <v>110</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Atelier A</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Fournisseur B</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2025-05-22</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>13.48</v>
-      </c>
-      <c r="H7" t="n">
-        <v>10</v>
-      </c>
-      <c r="I7" t="n">
-        <v>100</v>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-03-05</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Marteau 1kg</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>9384756201</v>
+      </c>
+      <c r="C13" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>60</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Atelier B</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Fournisseur C</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-03-04</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Perceuse filaire</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4758392016</v>
+      </c>
+      <c r="C14" t="n">
+        <v>25</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" t="n">
+        <v>50</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Atelier A</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Fournisseur A</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-03-03</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>69.98999999999999</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Vis 8x60mm</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>6574839201</v>
+      </c>
+      <c r="C15" t="n">
+        <v>800</v>
+      </c>
+      <c r="D15" t="n">
+        <v>80</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1600</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Stockage</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Fournisseur B</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-03-02</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Clé à pipe</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>3847562910</v>
+      </c>
+      <c r="C16" t="n">
+        <v>35</v>
+      </c>
+      <c r="D16" t="n">
+        <v>8</v>
+      </c>
+      <c r="E16" t="n">
+        <v>70</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Atelier B</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Fournisseur C</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-03-01</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>15.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification de l'interface utilisateur pour le niveau d'urgence dans la demande de matériel, passant d'un champ de texte à un bouton radio. Mise à jour de la gestion des données de demande pour refléter cette modification. Changement de l'affichage de l'urgence dans le récapitulatif de la demande. Mise à jour du fichier d'inventaire.
</commit_message>
<xml_diff>
--- a/data/inventaire.xlsx
+++ b/data/inventaire.xlsx
@@ -490,7 +490,7 @@
         <v>8473926150</v>
       </c>
       <c r="C2" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="n">
         <v>10</v>
@@ -601,7 +601,7 @@
         <v>5647382910</v>
       </c>
       <c r="C5" t="n">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D5" t="n">
         <v>100</v>
@@ -638,7 +638,7 @@
         <v>1928374650</v>
       </c>
       <c r="C6" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D6" t="n">
         <v>5</v>

</xml_diff>